<commit_message>
Rebalance stats and elements
</commit_message>
<xml_diff>
--- a/dev/stats.xlsx
+++ b/dev/stats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D6160B7A-4A2B-428F-9892-707E08500C09}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C722747F-D59C-4CAA-9AC6-4A404015E90D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -432,7 +432,7 @@
         <v>19</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>801</v>
@@ -455,7 +455,7 @@
         <v>20</v>
       </c>
       <c r="C3">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>756</v>
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>732</v>
@@ -501,7 +501,7 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>716</v>
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>698</v>
@@ -547,7 +547,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>654</v>
@@ -570,7 +570,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>648</v>
@@ -593,7 +593,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D9">
         <v>645</v>
@@ -616,7 +616,7 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>620</v>
@@ -630,7 +630,7 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>611</v>
@@ -644,7 +644,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>562</v>
@@ -658,7 +658,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D13">
         <v>559</v>
@@ -672,7 +672,7 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D14">
         <v>554</v>
@@ -686,7 +686,7 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>501</v>
@@ -700,7 +700,7 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>470</v>
@@ -738,19 +738,19 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D19">
-        <v>500</v>
+        <v>601</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
       </c>
       <c r="G19">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H19">
-        <v>453</v>
+        <v>574</v>
       </c>
       <c r="L19">
         <v>7</v>
@@ -767,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>331</v>
@@ -776,7 +776,7 @@
         <v>20</v>
       </c>
       <c r="G20">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H20">
         <v>346</v>
@@ -796,7 +796,7 @@
         <v>15</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D21">
         <v>301</v>
@@ -805,7 +805,7 @@
         <v>6</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H21">
         <v>310</v>
@@ -825,7 +825,7 @@
         <v>14</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D22">
         <v>299</v>
@@ -834,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H22">
         <v>304</v>
@@ -854,7 +854,7 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D23">
         <v>287</v>
@@ -863,7 +863,7 @@
         <v>7</v>
       </c>
       <c r="G23">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H23">
         <v>298</v>
@@ -883,7 +883,7 @@
         <v>13</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D24">
         <v>285</v>
@@ -892,7 +892,7 @@
         <v>13</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H24">
         <v>280</v>
@@ -912,7 +912,7 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D25">
         <v>276</v>
@@ -921,7 +921,7 @@
         <v>9</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H25">
         <v>273</v>
@@ -941,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D26">
         <v>265</v>
@@ -950,7 +950,7 @@
         <v>10</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H26">
         <v>268</v>
@@ -964,7 +964,7 @@
         <v>8</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D27">
         <v>255</v>
@@ -973,7 +973,7 @@
         <v>15</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H27">
         <v>252</v>
@@ -987,7 +987,7 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D28">
         <v>248</v>
@@ -996,7 +996,7 @@
         <v>14</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H28">
         <v>243</v>
@@ -1010,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D29">
         <v>242</v>
@@ -1019,7 +1019,7 @@
         <v>11</v>
       </c>
       <c r="G29">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H29">
         <v>215</v>
@@ -1033,7 +1033,7 @@
         <v>12</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D30">
         <v>218</v>
@@ -1042,10 +1042,10 @@
         <v>12</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H30">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -1056,7 +1056,7 @@
         <v>11</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D31">
         <v>189</v>
@@ -1065,10 +1065,10 @@
         <v>16</v>
       </c>
       <c r="G31">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H31">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -1079,7 +1079,7 @@
         <v>17</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>153</v>
@@ -1088,10 +1088,10 @@
         <v>17</v>
       </c>
       <c r="G32">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H32">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1102,7 +1102,7 @@
         <v>18</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D33">
         <v>151</v>
@@ -1111,10 +1111,10 @@
         <v>18</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H33">
-        <v>143</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1135,7 +1135,7 @@
         <v>18</v>
       </c>
       <c r="C36">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D36">
         <v>468</v>
@@ -1144,7 +1144,7 @@
         <v>14</v>
       </c>
       <c r="G36">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H36">
         <v>502</v>
@@ -1158,7 +1158,7 @@
         <v>17</v>
       </c>
       <c r="C37">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D37">
         <v>423</v>
@@ -1167,7 +1167,7 @@
         <v>15</v>
       </c>
       <c r="G37">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H37">
         <v>422</v>
@@ -1181,7 +1181,7 @@
         <v>12</v>
       </c>
       <c r="C38">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D38">
         <v>418</v>
@@ -1190,7 +1190,7 @@
         <v>16</v>
       </c>
       <c r="G38">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H38">
         <v>407</v>
@@ -1204,7 +1204,7 @@
         <v>11</v>
       </c>
       <c r="C39">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D39">
         <v>405</v>
@@ -1213,7 +1213,7 @@
         <v>13</v>
       </c>
       <c r="G39">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H39">
         <v>402</v>
@@ -1227,7 +1227,7 @@
         <v>10</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D40">
         <v>378</v>
@@ -1236,7 +1236,7 @@
         <v>19</v>
       </c>
       <c r="G40">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H40">
         <v>381</v>
@@ -1250,7 +1250,7 @@
         <v>7</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D41">
         <v>305</v>
@@ -1259,7 +1259,7 @@
         <v>9</v>
       </c>
       <c r="G41">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H41">
         <v>362</v>
@@ -1273,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D42">
         <v>301</v>
@@ -1282,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="G42">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H42">
         <v>350</v>
@@ -1296,7 +1296,7 @@
         <v>6</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D43">
         <v>298</v>
@@ -1305,7 +1305,7 @@
         <v>12</v>
       </c>
       <c r="G43">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H43">
         <v>332</v>
@@ -1319,7 +1319,7 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D44">
         <v>294</v>
@@ -1328,7 +1328,7 @@
         <v>18</v>
       </c>
       <c r="G44">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H44">
         <v>301</v>
@@ -1342,7 +1342,7 @@
         <v>19</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D45">
         <v>261</v>
@@ -1351,7 +1351,7 @@
         <v>17</v>
       </c>
       <c r="G45">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H45">
         <v>294</v>
@@ -1365,7 +1365,7 @@
         <v>16</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D46">
         <v>249</v>
@@ -1374,7 +1374,7 @@
         <v>20</v>
       </c>
       <c r="G46">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H46">
         <v>289</v>
@@ -1388,7 +1388,7 @@
         <v>15</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D47">
         <v>210</v>
@@ -1397,7 +1397,7 @@
         <v>7</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H47">
         <v>255</v>
@@ -1411,7 +1411,7 @@
         <v>14</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D48">
         <v>204</v>
@@ -1420,7 +1420,7 @@
         <v>6</v>
       </c>
       <c r="G48">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H48">
         <v>253</v>
@@ -1434,7 +1434,7 @@
         <v>13</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D49">
         <v>195</v>
@@ -1443,7 +1443,7 @@
         <v>11</v>
       </c>
       <c r="G49">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H49">
         <v>244</v>
@@ -1457,7 +1457,7 @@
         <v>20</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D50">
         <v>155</v>
@@ -1466,7 +1466,7 @@
         <v>8</v>
       </c>
       <c r="G50">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H50">
         <v>238</v>

</xml_diff>